<commit_message>
# Update Create TDGCRow form KQGCs
</commit_message>
<xml_diff>
--- a/ProcessManagement/wwwroot/ExportLocation/TDGCExcelForm.xlsx
+++ b/ProcessManagement/wwwroot/ExportLocation/TDGCExcelForm.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="TDGC" sheetId="1" r:id="rId1"/>
+    <sheet name="Tiện phi" sheetId="1" r:id="rId1"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId2"/>
@@ -15,7 +15,7 @@
   <definedNames>
     <definedName name="a"><![CDATA[[1]' '!$C$32:$E$67]]></definedName>
     <definedName name="af"><![CDATA[#REF!]]></definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA[TDGC!$B$1:$N$74]]></definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0"><![CDATA['Tiện phi'!$B$1:$N$74]]></definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="44">
   <si>
     <t xml:space="preserve">THEO DÕI TIẾN ĐỘ KẾ HOẠCH KIỂM HÀNG 200W</t>
   </si>
@@ -97,34 +97,79 @@
     <t xml:space="preserve">Ngày lập:  </t>
   </si>
   <si>
-    <t xml:space="preserve">THEO DÕI TIẾN ĐỘ KẾ HOẠCH KIỂM 100% REN RC 3/8 VBAT5A-1-7</t>
+    <t xml:space="preserve">THEO DÕI TIẾN ĐỘ KẾ HOẠCH TIỆN PHI P5053-1215-3</t>
   </si>
   <si>
     <t xml:space="preserve"/>
   </si>
   <si>
-    <t xml:space="preserve">VBAT5A-1-7</t>
+    <t xml:space="preserve">P5053-1215-3</t>
   </si>
   <si>
-    <t xml:space="preserve">Kiểm 100% ren RC 3/8</t>
+    <t xml:space="preserve">Tiện phi</t>
   </si>
   <si>
-    <t xml:space="preserve">B1</t>
+    <t xml:space="preserve">NC-14</t>
   </si>
   <si>
-    <t xml:space="preserve">Đêm</t>
+    <t xml:space="preserve">Văn Lâm</t>
   </si>
   <si>
-    <t xml:space="preserve">Hoàng Thuận</t>
+    <t xml:space="preserve">12.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hòa Đệ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7h-18h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quốc Việt</t>
   </si>
   <si>
     <t xml:space="preserve">0.00</t>
   </si>
   <si>
-    <t xml:space="preserve">Văn Lập, Hoàng Thuận</t>
+    <t xml:space="preserve">6h-14h</t>
   </si>
   <si>
-    <t xml:space="preserve">B2</t>
+    <t xml:space="preserve">11.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6h30-18h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Văn Giàu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8h-16h30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phước Vũ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6h-18h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7h30-18h</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dũ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NC-22</t>
   </si>
 </sst>
 </file>
@@ -1741,7 +1786,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="63">
-        <v>45741.659375</v>
+        <v>45765.51841435185</v>
       </c>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -1764,7 +1809,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="63">
-        <v>45747.659421296295</v>
+        <v>45770.518958333334</v>
       </c>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
@@ -1879,7 +1924,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="62">
-        <v>45744</v>
+        <v>45765.51841435185</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>21</v>
@@ -1891,28 +1936,28 @@
         <v>23</v>
       </c>
       <c r="F9" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="33">
+        <v>70</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="33">
-        <v>0</v>
-      </c>
-      <c r="H9" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9" s="34" t="s">
-        <v>25</v>
-      </c>
       <c r="J9" s="55">
-        <v>160</v>
+        <v>423</v>
       </c>
       <c r="K9" s="56">
-        <v>160</v>
+        <v>290</v>
       </c>
       <c r="L9" s="57">
         <v>0</v>
       </c>
       <c r="M9" s="56">
-        <v>0</v>
+        <v>-133</v>
       </c>
       <c r="N9" s="35" t="s">
         <v>20</v>
@@ -1932,7 +1977,7 @@
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="62">
-        <v>45744</v>
+        <v>45765.51841435185</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>21</v>
@@ -1941,31 +1986,31 @@
         <v>22</v>
       </c>
       <c r="E10" s="54" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F10" s="32" t="s">
         <v>4</v>
       </c>
       <c r="G10" s="33">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I10" s="34" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="J10" s="55">
-        <v>160</v>
+        <v>423</v>
       </c>
       <c r="K10" s="56">
-        <v>160</v>
+        <v>273</v>
       </c>
       <c r="L10" s="57">
         <v>0</v>
       </c>
       <c r="M10" s="56">
-        <v>0</v>
+        <v>-150</v>
       </c>
       <c r="N10" s="35" t="s">
         <v>20</v>
@@ -1982,7 +2027,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="62">
-        <v>45744</v>
+        <v>45759</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>21</v>
@@ -1991,25 +2036,25 @@
         <v>22</v>
       </c>
       <c r="E11" s="54" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F11" s="32" t="s">
         <v>4</v>
       </c>
       <c r="G11" s="33">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="H11" s="34" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I11" s="34" t="s">
         <v>27</v>
       </c>
       <c r="J11" s="55">
-        <v>160</v>
+        <v>379</v>
       </c>
       <c r="K11" s="56">
-        <v>160</v>
+        <v>379</v>
       </c>
       <c r="L11" s="57">
         <v>0</v>
@@ -2018,7 +2063,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="35" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="P11" s="36"/>
       <c r="Q11" s="37"/>
@@ -2032,7 +2077,7 @@
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12" s="62">
-        <v>45747</v>
+        <v>45759</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>21</v>
@@ -2041,25 +2086,25 @@
         <v>22</v>
       </c>
       <c r="E12" s="54" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F12" s="32" t="s">
         <v>4</v>
       </c>
       <c r="G12" s="33">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="H12" s="34" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I12" s="34" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J12" s="55">
-        <v>126</v>
+        <v>246</v>
       </c>
       <c r="K12" s="56">
-        <v>126</v>
+        <v>246</v>
       </c>
       <c r="L12" s="57">
         <v>0</v>
@@ -2068,7 +2113,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="35" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="P12" s="36"/>
       <c r="Q12" s="37"/>
@@ -2080,20 +2125,46 @@
       <c r="W12" s="12"/>
       <c r="Y12" s="5"/>
     </row>
-    <row r="13" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="62"/>
-      <c r="C13" s="32"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="57"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="35"/>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B13" s="62">
+        <v>45759</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="33">
+        <v>0</v>
+      </c>
+      <c r="H13" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="55">
+        <v>74</v>
+      </c>
+      <c r="K13" s="56">
+        <v>74</v>
+      </c>
+      <c r="L13" s="57">
+        <v>0</v>
+      </c>
+      <c r="M13" s="56">
+        <v>0</v>
+      </c>
+      <c r="N13" s="35" t="s">
+        <v>20</v>
+      </c>
       <c r="P13" s="36"/>
       <c r="Q13" s="37"/>
       <c r="R13" s="1"/>
@@ -2104,20 +2175,46 @@
       <c r="W13" s="12"/>
       <c r="Y13" s="5"/>
     </row>
-    <row r="14" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="62"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="54"/>
-      <c r="E14" s="54"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="57"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="35"/>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B14" s="62">
+        <v>45761</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="33">
+        <v>70</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="I14" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="55">
+        <v>40</v>
+      </c>
+      <c r="K14" s="56">
+        <v>40</v>
+      </c>
+      <c r="L14" s="57">
+        <v>0</v>
+      </c>
+      <c r="M14" s="56">
+        <v>0</v>
+      </c>
+      <c r="N14" s="35" t="s">
+        <v>34</v>
+      </c>
       <c r="P14" s="36"/>
       <c r="Q14" s="37"/>
       <c r="R14" s="1"/>
@@ -2128,20 +2225,46 @@
       <c r="W14" s="12"/>
       <c r="Y14" s="5"/>
     </row>
-    <row r="15" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="62"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="32"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="55"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="57"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="35"/>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="62">
+        <v>45761</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="33">
+        <v>70</v>
+      </c>
+      <c r="H15" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="I15" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="55">
+        <v>399</v>
+      </c>
+      <c r="K15" s="56">
+        <v>399</v>
+      </c>
+      <c r="L15" s="57">
+        <v>0</v>
+      </c>
+      <c r="M15" s="56">
+        <v>0</v>
+      </c>
+      <c r="N15" s="35" t="s">
+        <v>34</v>
+      </c>
       <c r="P15" s="36"/>
       <c r="Q15" s="37"/>
       <c r="R15" s="1"/>
@@ -2152,20 +2275,46 @@
       <c r="W15" s="12"/>
       <c r="Y15" s="5"/>
     </row>
-    <row r="16" spans="1:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="62"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
-      <c r="J16" s="55"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="35"/>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B16" s="62">
+        <v>45761</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="33">
+        <v>70</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="55">
+        <v>180</v>
+      </c>
+      <c r="K16" s="56">
+        <v>179</v>
+      </c>
+      <c r="L16" s="57">
+        <v>1</v>
+      </c>
+      <c r="M16" s="56">
+        <v>-1</v>
+      </c>
+      <c r="N16" s="35" t="s">
+        <v>37</v>
+      </c>
       <c r="P16" s="36"/>
       <c r="Q16" s="37"/>
       <c r="R16" s="1"/>
@@ -2176,20 +2325,46 @@
       <c r="W16" s="12"/>
       <c r="Y16" s="5"/>
     </row>
-    <row r="17" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="62"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="35"/>
+    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B17" s="62">
+        <v>45761</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="33">
+        <v>70</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="55">
+        <v>35</v>
+      </c>
+      <c r="K17" s="56">
+        <v>35</v>
+      </c>
+      <c r="L17" s="57">
+        <v>0</v>
+      </c>
+      <c r="M17" s="56">
+        <v>0</v>
+      </c>
+      <c r="N17" s="35" t="s">
+        <v>37</v>
+      </c>
       <c r="P17" s="36"/>
       <c r="Q17" s="37"/>
       <c r="R17" s="1"/>
@@ -2200,20 +2375,46 @@
       <c r="W17" s="12"/>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="62"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="35"/>
+    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B18" s="62">
+        <v>45762</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="33">
+        <v>70</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="J18" s="55">
+        <v>412</v>
+      </c>
+      <c r="K18" s="56">
+        <v>412</v>
+      </c>
+      <c r="L18" s="57">
+        <v>0</v>
+      </c>
+      <c r="M18" s="56">
+        <v>0</v>
+      </c>
+      <c r="N18" s="35" t="s">
+        <v>39</v>
+      </c>
       <c r="P18" s="36"/>
       <c r="Q18" s="37"/>
       <c r="R18" s="1"/>
@@ -2224,20 +2425,46 @@
       <c r="W18" s="12"/>
       <c r="Y18" s="5"/>
     </row>
-    <row r="19" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="62"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="55"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="35"/>
+    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B19" s="62">
+        <v>45762</v>
+      </c>
+      <c r="C19" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="33">
+        <v>70</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="J19" s="55">
+        <v>195</v>
+      </c>
+      <c r="K19" s="56">
+        <v>195</v>
+      </c>
+      <c r="L19" s="57">
+        <v>0</v>
+      </c>
+      <c r="M19" s="56">
+        <v>0</v>
+      </c>
+      <c r="N19" s="35" t="s">
+        <v>41</v>
+      </c>
       <c r="P19" s="36"/>
       <c r="Q19" s="37"/>
       <c r="R19" s="1"/>
@@ -2248,20 +2475,46 @@
       <c r="W19" s="12"/>
       <c r="Y19" s="5"/>
     </row>
-    <row r="20" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="62"/>
-      <c r="C20" s="32"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="35"/>
+    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B20" s="62">
+        <v>45763</v>
+      </c>
+      <c r="C20" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="33">
+        <v>70</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I20" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="55">
+        <v>412</v>
+      </c>
+      <c r="K20" s="56">
+        <v>411</v>
+      </c>
+      <c r="L20" s="57">
+        <v>1</v>
+      </c>
+      <c r="M20" s="56">
+        <v>-1</v>
+      </c>
+      <c r="N20" s="35" t="s">
+        <v>39</v>
+      </c>
       <c r="P20" s="36"/>
       <c r="Q20" s="37"/>
       <c r="R20" s="1"/>
@@ -2272,20 +2525,46 @@
       <c r="W20" s="12"/>
       <c r="Y20" s="5"/>
     </row>
-    <row r="21" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="62"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="54"/>
-      <c r="E21" s="54"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="55"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="35"/>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B21" s="62">
+        <v>45763</v>
+      </c>
+      <c r="C21" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="33">
+        <v>70</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="55">
+        <v>130</v>
+      </c>
+      <c r="K21" s="56">
+        <v>130</v>
+      </c>
+      <c r="L21" s="57">
+        <v>0</v>
+      </c>
+      <c r="M21" s="56">
+        <v>0</v>
+      </c>
+      <c r="N21" s="35" t="s">
+        <v>39</v>
+      </c>
       <c r="P21" s="36"/>
       <c r="Q21" s="37"/>
       <c r="R21" s="1"/>
@@ -2296,20 +2575,46 @@
       <c r="W21" s="12"/>
       <c r="Y21" s="5"/>
     </row>
-    <row r="22" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="62"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="54"/>
-      <c r="E22" s="54"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="55"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="57"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="35"/>
+    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B22" s="62">
+        <v>45763</v>
+      </c>
+      <c r="C22" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="33">
+        <v>70</v>
+      </c>
+      <c r="H22" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" s="55">
+        <v>135</v>
+      </c>
+      <c r="K22" s="56">
+        <v>135</v>
+      </c>
+      <c r="L22" s="57">
+        <v>0</v>
+      </c>
+      <c r="M22" s="56">
+        <v>0</v>
+      </c>
+      <c r="N22" s="35" t="s">
+        <v>39</v>
+      </c>
       <c r="P22" s="36"/>
       <c r="Q22" s="37"/>
       <c r="R22" s="1"/>
@@ -2320,20 +2625,46 @@
       <c r="W22" s="12"/>
       <c r="Y22" s="5"/>
     </row>
-    <row r="23" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="62"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="57"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="35"/>
+    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B23" s="62">
+        <v>45764</v>
+      </c>
+      <c r="C23" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="33">
+        <v>70</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="J23" s="55">
+        <v>145</v>
+      </c>
+      <c r="K23" s="56">
+        <v>145</v>
+      </c>
+      <c r="L23" s="57">
+        <v>0</v>
+      </c>
+      <c r="M23" s="56">
+        <v>0</v>
+      </c>
+      <c r="N23" s="35" t="s">
+        <v>39</v>
+      </c>
       <c r="P23" s="36"/>
       <c r="Q23" s="37"/>
       <c r="R23" s="1"/>
@@ -2344,20 +2675,46 @@
       <c r="W23" s="12"/>
       <c r="Y23" s="5"/>
     </row>
-    <row r="24" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="62"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="57"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="35"/>
+    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B24" s="62">
+        <v>45764</v>
+      </c>
+      <c r="C24" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="33">
+        <v>0</v>
+      </c>
+      <c r="H24" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="I24" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" s="55">
+        <v>295</v>
+      </c>
+      <c r="K24" s="56">
+        <v>295</v>
+      </c>
+      <c r="L24" s="57">
+        <v>0</v>
+      </c>
+      <c r="M24" s="56">
+        <v>0</v>
+      </c>
+      <c r="N24" s="35" t="s">
+        <v>20</v>
+      </c>
       <c r="P24" s="36"/>
       <c r="Q24" s="37"/>
       <c r="R24" s="1"/>
@@ -2368,20 +2725,46 @@
       <c r="W24" s="12"/>
       <c r="Y24" s="5"/>
     </row>
-    <row r="25" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="62"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="54"/>
-      <c r="E25" s="54"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="33"/>
-      <c r="H25" s="33"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="57"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="35"/>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="B25" s="62">
+        <v>45764</v>
+      </c>
+      <c r="C25" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="54" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="54" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="33">
+        <v>70</v>
+      </c>
+      <c r="H25" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" s="55">
+        <v>267</v>
+      </c>
+      <c r="K25" s="56">
+        <v>267</v>
+      </c>
+      <c r="L25" s="57">
+        <v>0</v>
+      </c>
+      <c r="M25" s="56">
+        <v>0</v>
+      </c>
+      <c r="N25" s="35" t="s">
+        <v>39</v>
+      </c>
       <c r="P25" s="36"/>
       <c r="Q25" s="37"/>
       <c r="R25" s="1"/>

</xml_diff>